<commit_message>
Updates to the presentaiton of data, the output files and the model
</commit_message>
<xml_diff>
--- a/SDG12_3/Excel/Indicator402B_2018-02-13.xlsx
+++ b/SDG12_3/Excel/Indicator402B_2018-02-13.xlsx
@@ -3917,7 +3917,7 @@
         <v>294</v>
       </c>
       <c r="C61" s="12" t="n">
-        <v>2.217</v>
+        <v>1.858</v>
       </c>
       <c r="D61" s="13" t="n">
         <f t="shared" si="0"/>
@@ -4160,7 +4160,7 @@
         <v>303</v>
       </c>
       <c r="C70" s="12" t="n">
-        <v>1.496</v>
+        <v>1.119</v>
       </c>
       <c r="D70" s="13" t="n">
         <f t="shared" si="4"/>
@@ -4295,7 +4295,7 @@
         <v>308</v>
       </c>
       <c r="C75" s="12" t="n">
-        <v>1.097</v>
+        <v>1.106</v>
       </c>
       <c r="D75" s="13" t="n">
         <f t="shared" si="4"/>
@@ -4322,7 +4322,7 @@
         <v>309</v>
       </c>
       <c r="C76" s="12" t="n">
-        <v>1.262</v>
+        <v>1.192</v>
       </c>
       <c r="D76" s="13" t="n">
         <f t="shared" si="4"/>
@@ -4619,7 +4619,7 @@
         <v>320</v>
       </c>
       <c r="C87" s="12" t="n">
-        <v>1.091</v>
+        <v>0.885</v>
       </c>
       <c r="D87" s="13" t="n">
         <f t="shared" si="4"/>
@@ -4700,7 +4700,7 @@
         <v>323</v>
       </c>
       <c r="C90" s="12" t="n">
-        <v>1.461</v>
+        <v>1.967</v>
       </c>
       <c r="D90" s="13" t="n">
         <f t="shared" si="4"/>
@@ -4727,7 +4727,7 @@
         <v>324</v>
       </c>
       <c r="C91" s="12" t="n">
-        <v>0.745</v>
+        <v>0.786</v>
       </c>
       <c r="D91" s="13" t="n">
         <f t="shared" si="4"/>
@@ -4916,7 +4916,7 @@
         <v>331</v>
       </c>
       <c r="C98" s="12" t="n">
-        <v>0.884</v>
+        <v>0.868</v>
       </c>
       <c r="D98" s="13" t="n">
         <f t="shared" si="4"/>
@@ -5051,7 +5051,7 @@
         <v>336</v>
       </c>
       <c r="C103" s="12" t="n">
-        <v>4.019</v>
+        <v>4.015</v>
       </c>
       <c r="D103" s="13" t="str">
         <f t="shared" si="4"/>
@@ -5321,7 +5321,7 @@
         <v>346</v>
       </c>
       <c r="C113" s="12" t="n">
-        <v>0.389</v>
+        <v>0.369</v>
       </c>
       <c r="D113" s="13" t="n">
         <f t="shared" si="4"/>
@@ -5564,7 +5564,7 @@
         <v>355</v>
       </c>
       <c r="C122" s="12" t="n">
-        <v>0.689</v>
+        <v>0.675</v>
       </c>
       <c r="D122" s="13" t="n">
         <f t="shared" si="4"/>

</xml_diff>